<commit_message>
Removed dir.h cuz io.h does the thing. Renamed files, functions and structs related to state search merge (since its rather easy to change between A*/BFS/DFS by changing priority in the state queue)
</commit_message>
<xml_diff>
--- a/build files and notes/build methods info.xlsx
+++ b/build files and notes/build methods info.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/585e6af98e7a4d57/Documents/C/C2export/build files and notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samo\OneDrive\Documents\C\C2export\build files and notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="351" documentId="8_{68C10737-5AD1-4342-B0FE-96908543E81E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8A38BFC8-A549-41EE-A2A9-C43662DB9963}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD961CF8-7E91-4F51-B567-489E8EA4402F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13224" yWindow="0" windowWidth="7656" windowHeight="4200" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
   <si>
     <t>0A</t>
   </si>
@@ -201,9 +202,6 @@
     <t>Occurence matrix (LL regeneration)</t>
   </si>
   <si>
-    <t>Occurence matrix  (no LL regeneration)</t>
-  </si>
-  <si>
     <t>21, 21, 21, 21, 21</t>
   </si>
   <si>
@@ -277,13 +275,19 @@
   </si>
   <si>
     <t>LL Gen. Settings</t>
+  </si>
+  <si>
+    <t>Xebra crash (mode 1), works elsewhere</t>
+  </si>
+  <si>
+    <t>Occurence matrix   (no LL regeneration)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +336,13 @@
       <charset val="238"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -424,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -433,17 +444,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -480,6 +480,70 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -492,62 +556,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -555,43 +564,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -720,23 +692,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -745,301 +745,324 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1049,11 +1072,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC00CC"/>
       <color rgb="FFFF7979"/>
       <color rgb="FFFF0000"/>
       <color rgb="FFFF5757"/>
       <color rgb="FF777777"/>
-      <color rgb="FFCC00CC"/>
       <color rgb="FFFF99FF"/>
       <color rgb="FFFF6600"/>
     </mruColors>
@@ -1368,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AD2FBA-18F5-4705-80AA-981EA7CD31DD}">
   <dimension ref="B1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,637 +1407,642 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="61"/>
+      <c r="B2" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="134" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="135"/>
+      <c r="J2" s="136"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="107" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="109"/>
+      <c r="H4" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="115"/>
+      <c r="J4" s="116"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="123" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="125"/>
+      <c r="H5" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="118"/>
+      <c r="J5" s="119"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="126" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="128"/>
+      <c r="H6" s="120" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="121"/>
+      <c r="J6" s="122"/>
+    </row>
+    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="142" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="104"/>
-      <c r="H4" s="109" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" s="110"/>
-      <c r="J4" s="111"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="118" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="120"/>
-      <c r="H5" s="112" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="113"/>
-      <c r="J5" s="114"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="121" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="123"/>
-      <c r="H6" s="115" t="s">
-        <v>74</v>
-      </c>
-      <c r="I6" s="116"/>
-      <c r="J6" s="117"/>
-    </row>
-    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="96" t="s">
+      <c r="C7" s="143"/>
+      <c r="D7" s="143"/>
+      <c r="E7" s="143"/>
+      <c r="F7" s="144"/>
+      <c r="H7" s="129" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="98"/>
-      <c r="H7" s="124" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="125"/>
-      <c r="J7" s="126"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="131"/>
     </row>
     <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="130" t="s">
+      <c r="B10" s="138" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="140" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="132" t="s">
+      <c r="D10" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="132" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="105" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="127" t="s">
+      <c r="E10" s="110" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="128"/>
-      <c r="H10" s="105" t="s">
+      <c r="G10" s="133"/>
+      <c r="H10" s="110" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="107" t="s">
+      <c r="J10" s="113"/>
+    </row>
+    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="139"/>
+      <c r="C11" s="141"/>
+      <c r="D11" s="141"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="108"/>
-    </row>
-    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="131"/>
-      <c r="C11" s="133"/>
-      <c r="D11" s="133"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="106"/>
-      <c r="I11" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="J11" s="81" t="s">
+      <c r="H11" s="111"/>
+      <c r="I11" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="69" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="82" t="s">
+      <c r="C12" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="84" t="s">
+      <c r="E12" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="85" t="s">
+      <c r="F12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="87" t="s">
         <v>48</v>
       </c>
       <c r="H12" s="74"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="77"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="65"/>
     </row>
     <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="63"/>
+      <c r="E13" s="85"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="36"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="31"/>
     </row>
     <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="87" t="s">
+      <c r="D14" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="88" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="19"/>
+      <c r="E14" s="86" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="14"/>
       <c r="G14" s="89"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="77"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="65"/>
     </row>
     <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="62" t="s">
+      <c r="E15" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="68" t="s">
+      <c r="F15" s="95" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="36"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="76"/>
     </row>
     <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="90" t="s">
+      <c r="C16" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="91" t="s">
+      <c r="D16" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="64"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="77"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="31"/>
     </row>
     <row r="17" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="84">
         <v>10</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="36"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="43">
         <v>11</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="68" t="s">
+      <c r="F18" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="H18" s="74"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="77"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="65"/>
     </row>
     <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="55">
+      <c r="D19" s="49">
         <v>12</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="36"/>
+      <c r="E19" s="97"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="43">
         <v>13</v>
       </c>
-      <c r="E20" s="62" t="s">
+      <c r="E20" s="98" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="68" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="74"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="77"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="65"/>
     </row>
     <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="35">
         <v>15</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="36"/>
+      <c r="E21" s="99"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="31"/>
     </row>
     <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="56">
+      <c r="D22" s="50">
         <v>16</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="77"/>
+      <c r="E22" s="99"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="65"/>
     </row>
     <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="35">
         <v>17</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="36"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="35">
         <v>18</v>
       </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="76"/>
-      <c r="J24" s="77"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="65"/>
     </row>
     <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="53">
+      <c r="D25" s="47">
         <v>19</v>
       </c>
-      <c r="E25" s="63"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="36"/>
+      <c r="E25" s="99"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="31"/>
     </row>
     <row r="26" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="D26" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="64"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="76"/>
-      <c r="J26" s="77"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="65"/>
     </row>
     <row r="27" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="36"/>
+      <c r="E27" s="99"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="64"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="77"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="65"/>
     </row>
     <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="65" t="s">
+      <c r="E29" s="101" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="70" t="s">
+      <c r="F29" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="32"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="31"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="H29" s="37"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="36"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="66" t="s">
+      <c r="F30" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" s="74"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="76"/>
+    </row>
+    <row r="31" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="10"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="100"/>
+      <c r="F31" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G30" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="H30" s="92"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="94"/>
-    </row>
-    <row r="31" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="13"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="16" t="s">
+      <c r="G31" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="G31" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="H31" s="75"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="79"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="67"/>
     </row>
     <row r="32" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="50" t="s">
+      <c r="C32" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="51">
+      <c r="D32" s="45">
         <v>20</v>
       </c>
-      <c r="E32" s="67"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="77"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="95"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="65"/>
     </row>
     <row r="33" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="50" t="s">
+      <c r="C33" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="51">
+      <c r="D33" s="45">
         <v>21</v>
       </c>
-      <c r="E33" s="67"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="36"/>
+      <c r="E33" s="92"/>
+      <c r="F33" s="95"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
     </row>
     <row r="34" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="8">
         <v>22</v>
       </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="77"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="64"/>
+      <c r="J34" s="65"/>
     </row>
     <row r="35" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="39">
+      <c r="D35" s="34">
         <v>23</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="36"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="31"/>
     </row>
     <row r="36" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="41">
+      <c r="D36" s="36">
         <v>24</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="77"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="91"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="65"/>
     </row>
     <row r="37" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="28" t="s">
         <v>39</v>
       </c>
       <c r="D37" s="4">
         <v>25</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="36"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="95"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="31"/>
     </row>
     <row r="38" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="47">
+      <c r="D38" s="42">
         <v>26</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="95"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="36"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="31"/>
     </row>
     <row r="39" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="44">
+      <c r="D39" s="39">
         <v>27</v>
       </c>
-      <c r="E39" s="59"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="78"/>
-      <c r="J39" s="79"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="91"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="63"/>
+      <c r="I39" s="66"/>
+      <c r="J39" s="67"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F40" s="129"/>
-      <c r="G40" s="129"/>
+      <c r="F40" s="137"/>
+      <c r="G40" s="137"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
@@ -2032,7 +2060,9 @@
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed config file, commented out unnecessary '#include's, in functions working with build's config array assigned necessary values to local variables with descriptive names
</commit_message>
<xml_diff>
--- a/build files and notes/build methods info.xlsx
+++ b/build files and notes/build methods info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samo\OneDrive\Documents\C\C2export\build files and notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD961CF8-7E91-4F51-B567-489E8EA4402F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F3D28F-B417-4ACE-AD26-E95506D0A403}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -947,6 +946,30 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1038,30 +1061,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1392,7 +1391,7 @@
   <dimension ref="B1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1407,117 +1406,117 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="112" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="106"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="114"/>
       <c r="G2" s="55"/>
-      <c r="H2" s="134" t="s">
+      <c r="H2" s="142" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="135"/>
-      <c r="J2" s="136"/>
+      <c r="I2" s="143"/>
+      <c r="J2" s="144"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="115" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="109"/>
-      <c r="H4" s="114" t="s">
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="117"/>
+      <c r="H4" s="122" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="115"/>
-      <c r="J4" s="116"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="124"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="131" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
-      <c r="F5" s="125"/>
-      <c r="H5" s="117" t="s">
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="133"/>
+      <c r="H5" s="125" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="118"/>
-      <c r="J5" s="119"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="127"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="134" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="128"/>
-      <c r="H6" s="120" t="s">
+      <c r="C6" s="135"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="136"/>
+      <c r="H6" s="128" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="121"/>
-      <c r="J6" s="122"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="130"/>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="142" t="s">
+      <c r="B7" s="109" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="143"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="143"/>
-      <c r="F7" s="144"/>
-      <c r="H7" s="129" t="s">
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="111"/>
+      <c r="H7" s="137" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="131"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="139"/>
     </row>
     <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="138" t="s">
+      <c r="B10" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="140" t="s">
+      <c r="C10" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="140" t="s">
+      <c r="D10" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="110" t="s">
+      <c r="E10" s="118" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="132" t="s">
+      <c r="F10" s="140" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="133"/>
-      <c r="H10" s="110" t="s">
+      <c r="G10" s="141"/>
+      <c r="H10" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="I10" s="112" t="s">
+      <c r="I10" s="120" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="113"/>
+      <c r="J10" s="121"/>
     </row>
     <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="139"/>
-      <c r="C11" s="141"/>
-      <c r="D11" s="141"/>
-      <c r="E11" s="111"/>
+      <c r="B11" s="106"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="119"/>
       <c r="F11" s="51" t="s">
         <v>79</v>
       </c>
       <c r="G11" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="111"/>
+      <c r="H11" s="119"/>
       <c r="I11" s="68" t="s">
         <v>79</v>
       </c>
@@ -2038,16 +2037,11 @@
       <c r="J39" s="67"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F40" s="137"/>
-      <c r="G40" s="137"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B7:F7"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H10:H11"/>
@@ -2061,6 +2055,11 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Replaced variable length arrays that didnt compile for older C standards with dynamically allocated ones
</commit_message>
<xml_diff>
--- a/build files and notes/build methods info.xlsx
+++ b/build files and notes/build methods info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samo\OneDrive\Documents\C\C2export\build files and notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F3D28F-B417-4ACE-AD26-E95506D0A403}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
@@ -946,30 +946,6 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1061,6 +1037,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1391,7 +1391,7 @@
   <dimension ref="B1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1406,117 +1406,117 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="114"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="106"/>
       <c r="G2" s="55"/>
-      <c r="H2" s="142" t="s">
+      <c r="H2" s="134" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="143"/>
-      <c r="J2" s="144"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="136"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="107" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="117"/>
-      <c r="H4" s="122" t="s">
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="109"/>
+      <c r="H4" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="123"/>
-      <c r="J4" s="124"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="116"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="123" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132"/>
-      <c r="F5" s="133"/>
-      <c r="H5" s="125" t="s">
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="125"/>
+      <c r="H5" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="126"/>
-      <c r="J5" s="127"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="119"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="134" t="s">
+      <c r="B6" s="126" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="136"/>
-      <c r="H6" s="128" t="s">
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="128"/>
+      <c r="H6" s="120" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="129"/>
-      <c r="J6" s="130"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="122"/>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="142" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="111"/>
-      <c r="H7" s="137" t="s">
+      <c r="C7" s="143"/>
+      <c r="D7" s="143"/>
+      <c r="E7" s="143"/>
+      <c r="F7" s="144"/>
+      <c r="H7" s="129" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="138"/>
-      <c r="J7" s="139"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="131"/>
     </row>
     <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="138" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="107" t="s">
+      <c r="C10" s="140" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="107" t="s">
+      <c r="D10" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="118" t="s">
+      <c r="E10" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="140" t="s">
+      <c r="F10" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="141"/>
-      <c r="H10" s="118" t="s">
+      <c r="G10" s="133"/>
+      <c r="H10" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="I10" s="120" t="s">
+      <c r="I10" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="121"/>
+      <c r="J10" s="113"/>
     </row>
     <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="106"/>
-      <c r="C11" s="108"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="119"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="141"/>
+      <c r="D11" s="141"/>
+      <c r="E11" s="111"/>
       <c r="F11" s="51" t="s">
         <v>79</v>
       </c>
       <c r="G11" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="119"/>
+      <c r="H11" s="111"/>
       <c r="I11" s="68" t="s">
         <v>79</v>
       </c>
@@ -2037,11 +2037,16 @@
       <c r="J39" s="67"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F40" s="104"/>
-      <c r="G40" s="104"/>
+      <c r="F40" s="137"/>
+      <c r="G40" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H10:H11"/>
@@ -2055,11 +2060,6 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>